<commit_message>
Unit Integration Skeleton Created
Unit Integration Skeleton Created and Tested Successfully. 6 September
2018
</commit_message>
<xml_diff>
--- a/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
+++ b/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Coach Number</t>
   </si>
@@ -41,7 +41,10 @@
     <t>2017-04-07</t>
   </si>
   <si>
-    <t>2017-04-12</t>
+    <t>2017-04-17</t>
+  </si>
+  <si>
+    <t>2017-04-16</t>
   </si>
 </sst>
 </file>
@@ -419,19 +422,19 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>13.56</v>
+        <v>7.0652</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -442,19 +445,19 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>7.0652</v>
+        <v>7.0026</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -474,7 +477,7 @@
         <v>7</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -497,7 +500,7 @@
         <v>7</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
User Role and User Account APIs created
User Role and User Account APIs created and tested successfully on 9
September 2018.
</commit_message>
<xml_diff>
--- a/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
+++ b/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Coach Number</t>
   </si>
@@ -38,13 +38,22 @@
     <t>Predicted Date of Failure</t>
   </si>
   <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>2017-04-07</t>
   </si>
   <si>
-    <t>2017-04-17</t>
-  </si>
-  <si>
-    <t>2017-04-16</t>
+    <t>2017-04-12</t>
+  </si>
+  <si>
+    <t>The Toe Creep has violated the wheel alarm settings thresholds</t>
+  </si>
+  <si>
+    <t>2017-04-11</t>
+  </si>
+  <si>
+    <t>The Flange Height has violated the wheel alarm settings thresholds</t>
   </si>
 </sst>
 </file>
@@ -383,7 +392,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -391,7 +400,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,8 +422,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>10805</v>
       </c>
@@ -428,16 +440,19 @@
         <v>7.0652</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>10805</v>
       </c>
@@ -451,16 +466,19 @@
         <v>7.0026</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F3">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>10805</v>
       </c>
@@ -474,16 +492,19 @@
         <v>7.1113</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>10805</v>
       </c>
@@ -497,16 +518,19 @@
         <v>7.1056</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>10805</v>
       </c>
@@ -520,13 +544,16 @@
         <v>32.9504</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wheel Measurements APIs created.
Wheel Measurements APIs created and successfully tested on 11 September
2018.
</commit_message>
<xml_diff>
--- a/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
+++ b/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Coach Number</t>
   </si>
@@ -42,15 +42,6 @@
   </si>
   <si>
     <t>2017-04-07</t>
-  </si>
-  <si>
-    <t>2017-04-12</t>
-  </si>
-  <si>
-    <t>The Toe Creep has violated the wheel alarm settings thresholds</t>
-  </si>
-  <si>
-    <t>2017-04-11</t>
   </si>
   <si>
     <t>The Flange Height has violated the wheel alarm settings thresholds</t>
@@ -437,19 +428,19 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>7.0652</v>
+        <v>30.1317</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -463,19 +454,19 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>7.0026</v>
+        <v>30.064</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -489,19 +480,19 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>7.1113</v>
+        <v>30.2994</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
         <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -515,19 +506,19 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>7.1056</v>
+        <v>30.0098</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
         <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -553,7 +544,7 @@
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created User Interface for Wheel Measurements
Created User Interface for Wheel Measurements and successfully Tested it
on 26 September 2018.
</commit_message>
<xml_diff>
--- a/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
+++ b/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>Coach Number</t>
   </si>
@@ -35,16 +35,7 @@
     <t>Number of Days before Failure</t>
   </si>
   <si>
-    <t>Predicted Date of Failure</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>2017-04-07</t>
-  </si>
-  <si>
-    <t>The Flange Height has violated the wheel alarm settings thresholds</t>
   </si>
 </sst>
 </file>
@@ -383,7 +374,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -391,7 +382,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,16 +401,10 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
-        <v>10805</v>
+        <v>12464</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -428,22 +413,16 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>30.1317</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>10805</v>
       </c>
@@ -451,51 +430,39 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>30.064</v>
+        <v>30.1317</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>10805</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4">
-        <v>30.2994</v>
+        <v>30.064</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>10805</v>
       </c>
@@ -503,25 +470,19 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>30.0098</v>
+        <v>30.2994</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>10805</v>
       </c>
@@ -535,16 +496,190 @@
         <v>32.9504</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>10805</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>-4.2395</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
         <v>0</v>
       </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>9</v>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>10805</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>32.1448</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>10805</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>33.4024</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>12464</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>31.2552</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>12464</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>30.1516</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>12464</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>6.6626</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12464</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>30.657</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>12464</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>30.2795</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>12464</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>30.2506</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Wheel Measurements User Interface
</commit_message>
<xml_diff>
--- a/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
+++ b/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>Coach Number</t>
   </si>
@@ -35,7 +35,70 @@
     <t>Number of Days before Failure</t>
   </si>
   <si>
+    <t>Predicted Date of Failure</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>2017-04-07</t>
+  </si>
+  <si>
+    <t>2017-12-19</t>
+  </si>
+  <si>
+    <t>The Flange Height has violated the wheel alarm settings thresholds</t>
+  </si>
+  <si>
+    <t>2017-12-22</t>
+  </si>
+  <si>
+    <t>2017-12-10</t>
+  </si>
+  <si>
+    <t>2017-07-23</t>
+  </si>
+  <si>
+    <t>The Hollowing has violated the wheel alarm settings thresholds</t>
+  </si>
+  <si>
+    <t>2017-09-04</t>
+  </si>
+  <si>
+    <t>2017-06-30</t>
+  </si>
+  <si>
+    <t>2017-10-21</t>
+  </si>
+  <si>
+    <t>2017-12-18</t>
+  </si>
+  <si>
+    <t>2017-08-15</t>
+  </si>
+  <si>
+    <t>The Toe Creep has violated the wheel alarm settings thresholds</t>
+  </si>
+  <si>
+    <t>2017-11-21</t>
+  </si>
+  <si>
+    <t>2017-12-11</t>
+  </si>
+  <si>
+    <t>2017-12-12</t>
+  </si>
+  <si>
+    <t>2017-07-16</t>
+  </si>
+  <si>
+    <t>2017-07-10</t>
+  </si>
+  <si>
+    <t>2017-09-19</t>
+  </si>
+  <si>
+    <t>2017-07-17</t>
   </si>
 </sst>
 </file>
@@ -374,7 +437,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -382,7 +445,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,10 +464,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
-        <v>12464</v>
+        <v>10805</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -413,16 +482,22 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>28</v>
+        <v>30.1317</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>256</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>10805</v>
       </c>
@@ -430,59 +505,77 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>30.1317</v>
+        <v>30.064</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F3">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>259</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>10805</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
-        <v>30.064</v>
+        <v>30.2994</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F4">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>247</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>10805</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>30.2994</v>
+        <v>32.9504</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>107</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>10805</v>
       </c>
@@ -490,39 +583,51 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>32.9504</v>
+        <v>-4.2395</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F6">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>10805</v>
       </c>
       <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
       <c r="D7">
-        <v>-4.2395</v>
+        <v>32.1448</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>150</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>10805</v>
       </c>
@@ -530,21 +635,27 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>32.1448</v>
+        <v>33.4024</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F8">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>84</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
-        <v>10805</v>
+        <v>12464</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -553,36 +664,48 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>33.4024</v>
+        <v>31.2552</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>197</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>12464</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>31.2552</v>
+        <v>30.1516</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F10">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>255</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>12464</v>
       </c>
@@ -590,39 +713,51 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>30.1516</v>
+        <v>6.6626</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F11">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>130</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>12464</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>6.6626</v>
+        <v>30.657</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F12">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>228</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>12464</v>
       </c>
@@ -630,39 +765,51 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13">
-        <v>30.657</v>
+        <v>30.2795</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>248</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>12464</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14">
-        <v>30.2795</v>
+        <v>30.2506</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F14">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>249</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>12464</v>
       </c>
@@ -670,16 +817,204 @@
         <v>4</v>
       </c>
       <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>6.6257</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>10810</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>33.2021</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>94</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>10810</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>31.8628</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>165</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>10810</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
         <v>7</v>
       </c>
-      <c r="D15">
-        <v>30.2506</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D18">
+        <v>33.0711</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>101</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>10810</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>33.2021</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>94</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>10810</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>33.2021</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>94</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>10810</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
         <v>6</v>
       </c>
-      <c r="F15">
-        <v>249</v>
+      <c r="D21">
+        <v>31.8628</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>165</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>10810</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>33.0711</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>101</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created Alarms and Reprofiling User Innterface
Created Alarms and Reprofiling User Innterface and tested successfully
on 28 September 2018.
</commit_message>
<xml_diff>
--- a/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
+++ b/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Coach Number</t>
   </si>
@@ -44,6 +44,12 @@
     <t>2017-04-07</t>
   </si>
   <si>
+    <t>The Cut Tyre Distance From Flange has violated the wheel alarm settings thresholds</t>
+  </si>
+  <si>
+    <t>The Gibson Ring has Failed it's inspection</t>
+  </si>
+  <si>
     <t>2017-12-19</t>
   </si>
   <si>
@@ -56,7 +62,7 @@
     <t>2017-12-10</t>
   </si>
   <si>
-    <t>2017-07-23</t>
+    <t>2017-12-25</t>
   </si>
   <si>
     <t>The Hollowing has violated the wheel alarm settings thresholds</t>
@@ -90,9 +96,6 @@
   </si>
   <si>
     <t>2017-07-16</t>
-  </si>
-  <si>
-    <t>2017-07-10</t>
   </si>
   <si>
     <t>2017-09-19</t>
@@ -437,7 +440,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,51 +476,51 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>10805</v>
+        <v>10810</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>30.1317</v>
+        <v>58.89</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2">
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>10805</v>
+        <v>10810</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>30.064</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3">
-        <v>259</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
@@ -525,25 +528,25 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>10805</v>
+        <v>10810</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>30.2994</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4">
-        <v>247</v>
+        <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -560,16 +563,16 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>32.9504</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -580,25 +583,25 @@
         <v>10805</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>-4.2395</v>
+        <v>30.1317</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -606,25 +609,25 @@
         <v>10805</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>32.1448</v>
+        <v>30.064</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
       <c r="F7">
-        <v>150</v>
+        <v>259</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -632,56 +635,56 @@
         <v>10805</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>33.4024</v>
+        <v>30.2994</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
       </c>
       <c r="F8">
-        <v>84</v>
+        <v>247</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
-        <v>12464</v>
+        <v>10805</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>31.2552</v>
+        <v>30.0098</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
       </c>
       <c r="F9">
-        <v>197</v>
+        <v>262</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
-        <v>12464</v>
+        <v>10805</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -690,71 +693,71 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>30.1516</v>
+        <v>-4.2395</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
-        <v>12464</v>
+        <v>10805</v>
       </c>
       <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
         <v>2</v>
       </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
       <c r="D11">
-        <v>6.6626</v>
+        <v>32.1448</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
       </c>
       <c r="F11">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
-        <v>12464</v>
+        <v>10805</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>30.657</v>
+        <v>33.4024</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="F12">
-        <v>228</v>
+        <v>84</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -762,25 +765,25 @@
         <v>12464</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>30.2795</v>
+        <v>31.2552</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13">
-        <v>248</v>
+        <v>197</v>
       </c>
       <c r="G13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -788,25 +791,25 @@
         <v>12464</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>30.2506</v>
+        <v>30.1516</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
       </c>
       <c r="F14">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -814,30 +817,30 @@
         <v>12464</v>
       </c>
       <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
         <v>4</v>
       </c>
-      <c r="C15">
-        <v>8</v>
-      </c>
       <c r="D15">
-        <v>6.6257</v>
+        <v>6.6626</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
       </c>
       <c r="F15">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="G15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16">
-        <v>10810</v>
+        <v>12464</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -846,24 +849,24 @@
         <v>5</v>
       </c>
       <c r="D16">
-        <v>33.2021</v>
+        <v>30.657</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16">
-        <v>94</v>
+        <v>228</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
-        <v>10810</v>
+        <v>12464</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -872,24 +875,24 @@
         <v>6</v>
       </c>
       <c r="D17">
-        <v>31.8628</v>
+        <v>30.2795</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17">
-        <v>165</v>
+        <v>248</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
-        <v>10810</v>
+        <v>12464</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -898,45 +901,45 @@
         <v>7</v>
       </c>
       <c r="D18">
-        <v>33.0711</v>
+        <v>30.2506</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
       </c>
       <c r="F18">
-        <v>101</v>
+        <v>249</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
-        <v>10810</v>
+        <v>12464</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>33.2021</v>
+        <v>6.6257</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
       </c>
       <c r="F19">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H19" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -947,22 +950,22 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20">
-        <v>33.2021</v>
+        <v>31.8628</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
       </c>
       <c r="F20">
-        <v>94</v>
+        <v>165</v>
       </c>
       <c r="G20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -970,25 +973,25 @@
         <v>10810</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D21">
-        <v>31.8628</v>
+        <v>33.0711</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
       </c>
       <c r="F21">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H21" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -996,25 +999,51 @@
         <v>10810</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22">
-        <v>33.0711</v>
+        <v>31.8628</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
       </c>
       <c r="F22">
-        <v>101</v>
+        <v>165</v>
       </c>
       <c r="G22" t="s">
         <v>27</v>
       </c>
       <c r="H22" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>10810</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>33.0711</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>101</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Manual Measurements User Interface
</commit_message>
<xml_diff>
--- a/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
+++ b/Eclipse Settings/WheelSystem/PlanningReport/report_305941_2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Coach Number</t>
   </si>
@@ -26,6 +26,9 @@
     <t>Wheel ID</t>
   </si>
   <si>
+    <t>Wheel Size</t>
+  </si>
+  <si>
     <t>Defect Size (mm)</t>
   </si>
   <si>
@@ -41,10 +44,16 @@
     <t>Comment</t>
   </si>
   <si>
+    <t>73.25 in</t>
+  </si>
+  <si>
     <t>2017-04-07</t>
   </si>
   <si>
     <t>The Flange Height has violated the wheel alarm settings thresholds</t>
+  </si>
+  <si>
+    <t>0 mm</t>
   </si>
 </sst>
 </file>
@@ -383,7 +392,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -391,7 +400,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,34 +425,40 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>10805</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>30.1317</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>30.2994</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>10805</v>
       </c>
@@ -451,51 +466,57 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>30.064</v>
-      </c>
-      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F3">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>30.1317</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>10805</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>30.2994</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>30.064</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>10805</v>
       </c>
@@ -505,23 +526,26 @@
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
         <v>30.0098</v>
       </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
         <v>0</v>
       </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>10805</v>
       </c>
@@ -531,20 +555,23 @@
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6">
         <v>32.9504</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
         <v>0</v>
       </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
       <c r="H6" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>